<commit_message>
Update README.md, transformacion_dataset_terremotos e inclusion de nuevos csv
</commit_message>
<xml_diff>
--- a/files/Campos_del_dataframe_terremotos.xlsx
+++ b/files/Campos_del_dataframe_terremotos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Clasificacion del terremoto en base a su magnitud</t>
   </si>
   <si>
-    <t>Tipo</t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
@@ -185,6 +182,36 @@
   </si>
   <si>
     <t>Hora de inclusion del terremoto en los ficheros</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>latitud_entero</t>
+  </si>
+  <si>
+    <t>longitud_entero</t>
+  </si>
+  <si>
+    <t>coordenadas</t>
+  </si>
+  <si>
+    <t>paises</t>
+  </si>
+  <si>
+    <t>Zona geografica donde se produce el terremoto, formato corto</t>
+  </si>
+  <si>
+    <t>Latitud expresada indicando solo el entero (sin decimales)</t>
+  </si>
+  <si>
+    <t>Longitud expresada indicando solo el entero (sin decimales)</t>
+  </si>
+  <si>
+    <t>Columna donde se indica latitud y longitud en valor entero separados por una coma</t>
+  </si>
+  <si>
+    <t>País donde se produce el terremoto</t>
   </si>
 </sst>
 </file>
@@ -540,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,7 +587,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -571,7 +598,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -582,7 +609,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -593,7 +620,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -602,7 +629,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -613,7 +640,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -624,7 +651,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -635,7 +662,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -646,7 +673,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -657,7 +684,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -668,7 +695,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -679,7 +706,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -688,7 +715,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -699,159 +726,214 @@
         <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>28</v>
+      <c r="B29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>